<commit_message>
Implemented an operational  webpage
</commit_message>
<xml_diff>
--- a/eeprom_map_n_pin_layout.xlsx
+++ b/eeprom_map_n_pin_layout.xlsx
@@ -9,13 +9,14 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="5940"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="5940" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="EEPROM" sheetId="1" r:id="rId1"/>
     <sheet name="GPIO" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="152511"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="68">
   <si>
     <t>Partition 1</t>
   </si>
@@ -225,7 +226,10 @@
     <t>no pull down at boot</t>
   </si>
   <si>
-    <t>Light index relative to this button  [(1 - 5)] (5 output pins), [0xFE] dimmer selector, [0xFF] disabled</t>
+    <t>Light index relative to this button  [(1 - 5)] (5 output pins), [0xC8] dimmer selector, [0xFE] software disabled, [0xFF] disabled</t>
+  </si>
+  <si>
+    <t>No dimmer</t>
   </si>
 </sst>
 </file>
@@ -720,8 +724,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AN48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="P1" workbookViewId="0">
-      <selection activeCell="AI20" sqref="AI20:AN25"/>
+    <sheetView topLeftCell="P1" workbookViewId="0">
+      <selection activeCell="AI14" sqref="AI14:AN19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2853,8 +2857,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M19" sqref="M19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3090,6 +3094,9 @@
       <c r="C12" t="s">
         <v>61</v>
       </c>
+      <c r="D12" t="s">
+        <v>67</v>
+      </c>
       <c r="E12" t="s">
         <v>62</v>
       </c>

</xml_diff>

<commit_message>
Implement web page interaction, & correct bugs
</commit_message>
<xml_diff>
--- a/eeprom_map_n_pin_layout.xlsx
+++ b/eeprom_map_n_pin_layout.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="73">
   <si>
     <t>Partition 1</t>
   </si>
@@ -230,6 +230,21 @@
   </si>
   <si>
     <t>No dimmer</t>
+  </si>
+  <si>
+    <t>amarelo</t>
+  </si>
+  <si>
+    <t>azul</t>
+  </si>
+  <si>
+    <t>laranja</t>
+  </si>
+  <si>
+    <t>verde</t>
+  </si>
+  <si>
+    <t>roxo</t>
   </si>
 </sst>
 </file>
@@ -2858,7 +2873,7 @@
   <dimension ref="A1:L18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M19" sqref="M19"/>
+      <selection activeCell="M20" sqref="M20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2901,6 +2916,9 @@
       <c r="E2" t="s">
         <v>56</v>
       </c>
+      <c r="F2" t="s">
+        <v>68</v>
+      </c>
       <c r="I2" s="22"/>
       <c r="J2" s="23">
         <v>1</v>
@@ -2962,6 +2980,9 @@
       <c r="E5" t="s">
         <v>56</v>
       </c>
+      <c r="F5" t="s">
+        <v>69</v>
+      </c>
       <c r="I5" s="21"/>
       <c r="J5" s="23"/>
       <c r="K5" s="23"/>
@@ -3005,6 +3026,9 @@
       <c r="E7" t="s">
         <v>56</v>
       </c>
+      <c r="F7" t="s">
+        <v>70</v>
+      </c>
       <c r="I7" s="21"/>
       <c r="J7" s="23"/>
       <c r="K7" s="23"/>
@@ -3172,7 +3196,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>15</v>
       </c>
@@ -3182,8 +3206,11 @@
       <c r="E17" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F17" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>16</v>
       </c>
@@ -3192,6 +3219,9 @@
       </c>
       <c r="E18" t="s">
         <v>56</v>
+      </c>
+      <c r="F18" t="s">
+        <v>72</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Main & Lighter code revised. Changed webserver routes
</commit_message>
<xml_diff>
--- a/eeprom_map_n_pin_layout.xlsx
+++ b/eeprom_map_n_pin_layout.xlsx
@@ -9,14 +9,14 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="5940" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="5940" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="EEPROM" sheetId="1" r:id="rId1"/>
     <sheet name="GPIO" sheetId="2" r:id="rId2"/>
+    <sheet name="Light mode" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="152511"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="191" uniqueCount="88">
   <si>
     <t>Partition 1</t>
   </si>
@@ -109,9 +109,6 @@
     <t>Light dimmer 6</t>
   </si>
   <si>
-    <t>Configured dimmer (1 - 254 ) -&gt; (1% - 100%)</t>
-  </si>
-  <si>
     <t>Access Point (0), WiFi Client (1)</t>
   </si>
   <si>
@@ -160,9 +157,6 @@
     <t>BTN logic level</t>
   </si>
   <si>
-    <t>Set button initial (not touched) logic level (HIGH/LOW)</t>
-  </si>
-  <si>
     <t>Manager port MSB</t>
   </si>
   <si>
@@ -226,9 +220,6 @@
     <t>no pull down at boot</t>
   </si>
   <si>
-    <t>Light index relative to this button  [(1 - 5)] (5 output pins), [0xC8] dimmer selector, [0xFE] software disabled, [0xFF] disabled</t>
-  </si>
-  <si>
     <t>No dimmer</t>
   </si>
   <si>
@@ -244,7 +235,61 @@
     <t>verde</t>
   </si>
   <si>
-    <t>roxo</t>
+    <t>Set button initial (not touched) logic level (HIGH/LOW) [HIGH]</t>
+  </si>
+  <si>
+    <t>Configured dimmer (1 - 100) -&gt; (1% - 100%)</t>
+  </si>
+  <si>
+    <t>roxo/marrom</t>
+  </si>
+  <si>
+    <t>Value</t>
+  </si>
+  <si>
+    <t>Decription</t>
+  </si>
+  <si>
+    <t>0XFA</t>
+  </si>
+  <si>
+    <t>0xFE</t>
+  </si>
+  <si>
+    <t>0XFF</t>
+  </si>
+  <si>
+    <t>Connected to output 1</t>
+  </si>
+  <si>
+    <t>Connected to output 2</t>
+  </si>
+  <si>
+    <t>Connected to output 3</t>
+  </si>
+  <si>
+    <t>Connected to output 4</t>
+  </si>
+  <si>
+    <t>Connected to output 5</t>
+  </si>
+  <si>
+    <t>Not configured</t>
+  </si>
+  <si>
+    <t>Disabled by software. Software may disable button for some reason (other button holded for exemple)</t>
+  </si>
+  <si>
+    <t>Disabled</t>
+  </si>
+  <si>
+    <t>Light index relative to this button. See Light mode table for details</t>
+  </si>
+  <si>
+    <t>0xC8</t>
+  </si>
+  <si>
+    <t>Dimmer</t>
   </si>
 </sst>
 </file>
@@ -415,7 +460,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -441,6 +486,9 @@
     <xf numFmtId="0" fontId="0" fillId="21" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -739,8 +787,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AN48"/>
   <sheetViews>
-    <sheetView topLeftCell="P1" workbookViewId="0">
-      <selection activeCell="AI14" sqref="AI14:AN19"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="AQ14" sqref="AQ14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -827,17 +875,17 @@
       <c r="Y1" s="20">
         <v>24</v>
       </c>
-      <c r="Z1" s="25" t="s">
+      <c r="Z1" s="26" t="s">
         <v>0</v>
       </c>
-      <c r="AB1" s="27" t="s">
+      <c r="AB1" s="28" t="s">
         <v>0</v>
       </c>
-      <c r="AC1" s="27"/>
-      <c r="AE1" s="27" t="s">
+      <c r="AC1" s="28"/>
+      <c r="AE1" s="28" t="s">
         <v>1</v>
       </c>
-      <c r="AF1" s="27"/>
+      <c r="AF1" s="28"/>
     </row>
     <row r="2" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A2">
@@ -915,27 +963,27 @@
       <c r="Y2">
         <v>49</v>
       </c>
-      <c r="Z2" s="25"/>
+      <c r="Z2" s="26"/>
       <c r="AB2" s="14" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="AC2" t="s">
         <v>5</v>
       </c>
       <c r="AE2" s="9" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="AF2" t="s">
         <v>5</v>
       </c>
-      <c r="AI2" s="24" t="s">
-        <v>28</v>
-      </c>
-      <c r="AJ2" s="24"/>
-      <c r="AK2" s="24"/>
-      <c r="AL2" s="24"/>
-      <c r="AM2" s="24"/>
-      <c r="AN2" s="24"/>
+      <c r="AI2" s="25" t="s">
+        <v>27</v>
+      </c>
+      <c r="AJ2" s="25"/>
+      <c r="AK2" s="25"/>
+      <c r="AL2" s="25"/>
+      <c r="AM2" s="25"/>
+      <c r="AN2" s="25"/>
     </row>
     <row r="3" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A3" s="4">
@@ -1013,27 +1061,27 @@
       <c r="Y3" s="4">
         <v>74</v>
       </c>
-      <c r="Z3" s="25"/>
+      <c r="Z3" s="26"/>
       <c r="AB3" s="14" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="AC3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="AE3" s="9" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="AF3" t="s">
-        <v>43</v>
-      </c>
-      <c r="AI3" s="24" t="s">
-        <v>44</v>
-      </c>
-      <c r="AJ3" s="24"/>
-      <c r="AK3" s="24"/>
-      <c r="AL3" s="24"/>
-      <c r="AM3" s="24"/>
-      <c r="AN3" s="24"/>
+        <v>42</v>
+      </c>
+      <c r="AI3" s="25" t="s">
+        <v>69</v>
+      </c>
+      <c r="AJ3" s="25"/>
+      <c r="AK3" s="25"/>
+      <c r="AL3" s="25"/>
+      <c r="AM3" s="25"/>
+      <c r="AN3" s="25"/>
     </row>
     <row r="4" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A4" s="4">
@@ -1111,12 +1159,12 @@
       <c r="Y4" s="4">
         <v>99</v>
       </c>
-      <c r="Z4" s="25"/>
+      <c r="Z4" s="26"/>
       <c r="AB4" s="14" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="AE4" s="9" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="5" spans="1:40" x14ac:dyDescent="0.25">
@@ -1195,12 +1243,12 @@
       <c r="Y5" s="4">
         <v>124</v>
       </c>
-      <c r="Z5" s="25"/>
+      <c r="Z5" s="26"/>
       <c r="AB5" s="14" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="AE5" s="9" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="6" spans="1:40" x14ac:dyDescent="0.25">
@@ -1279,12 +1327,12 @@
       <c r="Y6" s="4">
         <v>149</v>
       </c>
-      <c r="Z6" s="25"/>
+      <c r="Z6" s="26"/>
       <c r="AB6" s="14" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="AE6" s="9" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="7" spans="1:40" x14ac:dyDescent="0.25">
@@ -1363,12 +1411,12 @@
       <c r="Y7" s="3">
         <v>174</v>
       </c>
-      <c r="Z7" s="25"/>
+      <c r="Z7" s="26"/>
       <c r="AB7" s="14" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="AE7" s="9" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="8" spans="1:40" x14ac:dyDescent="0.25">
@@ -1447,12 +1495,12 @@
       <c r="Y8" s="3">
         <v>199</v>
       </c>
-      <c r="Z8" s="25"/>
+      <c r="Z8" s="26"/>
       <c r="AB8" s="14" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="AE8" s="9" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="9" spans="1:40" x14ac:dyDescent="0.25">
@@ -1531,12 +1579,12 @@
       <c r="Y9" s="3">
         <v>224</v>
       </c>
-      <c r="Z9" s="25"/>
+      <c r="Z9" s="26"/>
       <c r="AB9" s="14" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="AE9" s="9" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="10" spans="1:40" x14ac:dyDescent="0.25">
@@ -1615,27 +1663,27 @@
       <c r="Y10" s="3">
         <v>249</v>
       </c>
-      <c r="Z10" s="25"/>
+      <c r="Z10" s="26"/>
       <c r="AB10" s="11" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="AC10" t="s">
         <v>6</v>
       </c>
       <c r="AE10" s="6" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="AF10" t="s">
         <v>6</v>
       </c>
-      <c r="AI10" s="24" t="s">
+      <c r="AI10" s="25" t="s">
         <v>10</v>
       </c>
-      <c r="AJ10" s="24"/>
-      <c r="AK10" s="24"/>
-      <c r="AL10" s="24"/>
-      <c r="AM10" s="24"/>
-      <c r="AN10" s="24"/>
+      <c r="AJ10" s="25"/>
+      <c r="AK10" s="25"/>
+      <c r="AL10" s="25"/>
+      <c r="AM10" s="25"/>
+      <c r="AN10" s="25"/>
     </row>
     <row r="11" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A11" s="9">
@@ -1713,29 +1761,29 @@
       <c r="Y11">
         <v>274</v>
       </c>
-      <c r="Z11" s="25" t="s">
+      <c r="Z11" s="26" t="s">
         <v>1</v>
       </c>
       <c r="AB11" s="10" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="AC11" t="s">
         <v>12</v>
       </c>
       <c r="AE11" s="17" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="AF11" t="s">
         <v>12</v>
       </c>
-      <c r="AI11" s="24" t="s">
+      <c r="AI11" s="25" t="s">
         <v>11</v>
       </c>
-      <c r="AJ11" s="24"/>
-      <c r="AK11" s="24"/>
-      <c r="AL11" s="24"/>
-      <c r="AM11" s="24"/>
-      <c r="AN11" s="24"/>
+      <c r="AJ11" s="25"/>
+      <c r="AK11" s="25"/>
+      <c r="AL11" s="25"/>
+      <c r="AM11" s="25"/>
+      <c r="AN11" s="25"/>
     </row>
     <row r="12" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A12">
@@ -1813,7 +1861,7 @@
       <c r="Y12">
         <v>299</v>
       </c>
-      <c r="Z12" s="25"/>
+      <c r="Z12" s="26"/>
     </row>
     <row r="13" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A13" s="5">
@@ -1891,7 +1939,7 @@
       <c r="Y13" s="5">
         <v>324</v>
       </c>
-      <c r="Z13" s="25"/>
+      <c r="Z13" s="26"/>
     </row>
     <row r="14" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A14" s="5">
@@ -1969,27 +2017,27 @@
       <c r="Y14" s="5">
         <v>349</v>
       </c>
-      <c r="Z14" s="25"/>
+      <c r="Z14" s="26"/>
       <c r="AB14" s="16" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="AC14" t="s">
         <v>15</v>
       </c>
       <c r="AE14" s="8" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="AF14" t="s">
         <v>15</v>
       </c>
-      <c r="AI14" s="28" t="s">
-        <v>66</v>
-      </c>
-      <c r="AJ14" s="28"/>
-      <c r="AK14" s="28"/>
-      <c r="AL14" s="28"/>
-      <c r="AM14" s="28"/>
-      <c r="AN14" s="28"/>
+      <c r="AI14" s="29" t="s">
+        <v>85</v>
+      </c>
+      <c r="AJ14" s="29"/>
+      <c r="AK14" s="29"/>
+      <c r="AL14" s="29"/>
+      <c r="AM14" s="29"/>
+      <c r="AN14" s="29"/>
     </row>
     <row r="15" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A15" s="5">
@@ -2067,25 +2115,25 @@
       <c r="Y15" s="5">
         <v>374</v>
       </c>
-      <c r="Z15" s="25"/>
+      <c r="Z15" s="26"/>
       <c r="AB15" s="16" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="AC15" t="s">
         <v>16</v>
       </c>
       <c r="AE15" s="8" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="AF15" t="s">
         <v>16</v>
       </c>
-      <c r="AI15" s="28"/>
-      <c r="AJ15" s="28"/>
-      <c r="AK15" s="28"/>
-      <c r="AL15" s="28"/>
-      <c r="AM15" s="28"/>
-      <c r="AN15" s="28"/>
+      <c r="AI15" s="29"/>
+      <c r="AJ15" s="29"/>
+      <c r="AK15" s="29"/>
+      <c r="AL15" s="29"/>
+      <c r="AM15" s="29"/>
+      <c r="AN15" s="29"/>
     </row>
     <row r="16" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A16" s="5">
@@ -2163,25 +2211,25 @@
       <c r="Y16" s="5">
         <v>399</v>
       </c>
-      <c r="Z16" s="25"/>
+      <c r="Z16" s="26"/>
       <c r="AB16" s="16" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="AC16" t="s">
         <v>17</v>
       </c>
       <c r="AE16" s="8" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="AF16" t="s">
         <v>17</v>
       </c>
-      <c r="AI16" s="28"/>
-      <c r="AJ16" s="28"/>
-      <c r="AK16" s="28"/>
-      <c r="AL16" s="28"/>
-      <c r="AM16" s="28"/>
-      <c r="AN16" s="28"/>
+      <c r="AI16" s="29"/>
+      <c r="AJ16" s="29"/>
+      <c r="AK16" s="29"/>
+      <c r="AL16" s="29"/>
+      <c r="AM16" s="29"/>
+      <c r="AN16" s="29"/>
     </row>
     <row r="17" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A17" s="2">
@@ -2259,25 +2307,25 @@
       <c r="Y17" s="2">
         <v>424</v>
       </c>
-      <c r="Z17" s="25"/>
+      <c r="Z17" s="26"/>
       <c r="AB17" s="16" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="AC17" t="s">
         <v>18</v>
       </c>
       <c r="AE17" s="8" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="AF17" t="s">
         <v>18</v>
       </c>
-      <c r="AI17" s="28"/>
-      <c r="AJ17" s="28"/>
-      <c r="AK17" s="28"/>
-      <c r="AL17" s="28"/>
-      <c r="AM17" s="28"/>
-      <c r="AN17" s="28"/>
+      <c r="AI17" s="29"/>
+      <c r="AJ17" s="29"/>
+      <c r="AK17" s="29"/>
+      <c r="AL17" s="29"/>
+      <c r="AM17" s="29"/>
+      <c r="AN17" s="29"/>
     </row>
     <row r="18" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A18" s="2">
@@ -2355,25 +2403,25 @@
       <c r="Y18" s="2">
         <v>449</v>
       </c>
-      <c r="Z18" s="25"/>
+      <c r="Z18" s="26"/>
       <c r="AB18" s="16" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="AC18" t="s">
         <v>19</v>
       </c>
       <c r="AE18" s="8" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="AF18" t="s">
         <v>19</v>
       </c>
-      <c r="AI18" s="28"/>
-      <c r="AJ18" s="28"/>
-      <c r="AK18" s="28"/>
-      <c r="AL18" s="28"/>
-      <c r="AM18" s="28"/>
-      <c r="AN18" s="28"/>
+      <c r="AI18" s="29"/>
+      <c r="AJ18" s="29"/>
+      <c r="AK18" s="29"/>
+      <c r="AL18" s="29"/>
+      <c r="AM18" s="29"/>
+      <c r="AN18" s="29"/>
     </row>
     <row r="19" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A19" s="2">
@@ -2451,25 +2499,25 @@
       <c r="Y19" s="2">
         <v>474</v>
       </c>
-      <c r="Z19" s="25"/>
+      <c r="Z19" s="26"/>
       <c r="AB19" s="16" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="AC19" t="s">
         <v>20</v>
       </c>
       <c r="AE19" s="8" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="AF19" t="s">
         <v>20</v>
       </c>
-      <c r="AI19" s="28"/>
-      <c r="AJ19" s="28"/>
-      <c r="AK19" s="28"/>
-      <c r="AL19" s="28"/>
-      <c r="AM19" s="28"/>
-      <c r="AN19" s="28"/>
+      <c r="AI19" s="29"/>
+      <c r="AJ19" s="29"/>
+      <c r="AK19" s="29"/>
+      <c r="AL19" s="29"/>
+      <c r="AM19" s="29"/>
+      <c r="AN19" s="29"/>
     </row>
     <row r="20" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A20" s="2">
@@ -2547,27 +2595,27 @@
       <c r="Y20" s="2">
         <v>499</v>
       </c>
-      <c r="Z20" s="25"/>
+      <c r="Z20" s="26"/>
       <c r="AB20" s="15" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="AC20" t="s">
         <v>21</v>
       </c>
       <c r="AE20" s="7" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="AF20" t="s">
         <v>21</v>
       </c>
-      <c r="AI20" s="26" t="s">
-        <v>27</v>
-      </c>
-      <c r="AJ20" s="26"/>
-      <c r="AK20" s="26"/>
-      <c r="AL20" s="26"/>
-      <c r="AM20" s="26"/>
-      <c r="AN20" s="26"/>
+      <c r="AI20" s="27" t="s">
+        <v>70</v>
+      </c>
+      <c r="AJ20" s="27"/>
+      <c r="AK20" s="27"/>
+      <c r="AL20" s="27"/>
+      <c r="AM20" s="27"/>
+      <c r="AN20" s="27"/>
     </row>
     <row r="21" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A21">
@@ -2607,177 +2655,177 @@
         <v>511</v>
       </c>
       <c r="AB21" s="15" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="AC21" t="s">
         <v>22</v>
       </c>
       <c r="AE21" s="7" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="AF21" t="s">
         <v>22</v>
       </c>
-      <c r="AI21" s="26"/>
-      <c r="AJ21" s="26"/>
-      <c r="AK21" s="26"/>
-      <c r="AL21" s="26"/>
-      <c r="AM21" s="26"/>
-      <c r="AN21" s="26"/>
+      <c r="AI21" s="27"/>
+      <c r="AJ21" s="27"/>
+      <c r="AK21" s="27"/>
+      <c r="AL21" s="27"/>
+      <c r="AM21" s="27"/>
+      <c r="AN21" s="27"/>
     </row>
     <row r="22" spans="1:40" x14ac:dyDescent="0.25">
       <c r="AB22" s="15" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="AC22" t="s">
         <v>23</v>
       </c>
       <c r="AE22" s="7" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="AF22" t="s">
         <v>23</v>
       </c>
-      <c r="AI22" s="26"/>
-      <c r="AJ22" s="26"/>
-      <c r="AK22" s="26"/>
-      <c r="AL22" s="26"/>
-      <c r="AM22" s="26"/>
-      <c r="AN22" s="26"/>
+      <c r="AI22" s="27"/>
+      <c r="AJ22" s="27"/>
+      <c r="AK22" s="27"/>
+      <c r="AL22" s="27"/>
+      <c r="AM22" s="27"/>
+      <c r="AN22" s="27"/>
     </row>
     <row r="23" spans="1:40" x14ac:dyDescent="0.25">
       <c r="AB23" s="15" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="AC23" t="s">
         <v>24</v>
       </c>
       <c r="AE23" s="7" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="AF23" t="s">
         <v>24</v>
       </c>
-      <c r="AI23" s="26"/>
-      <c r="AJ23" s="26"/>
-      <c r="AK23" s="26"/>
-      <c r="AL23" s="26"/>
-      <c r="AM23" s="26"/>
-      <c r="AN23" s="26"/>
+      <c r="AI23" s="27"/>
+      <c r="AJ23" s="27"/>
+      <c r="AK23" s="27"/>
+      <c r="AL23" s="27"/>
+      <c r="AM23" s="27"/>
+      <c r="AN23" s="27"/>
     </row>
     <row r="24" spans="1:40" x14ac:dyDescent="0.25">
       <c r="W24" s="1"/>
       <c r="AB24" s="15" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="AC24" t="s">
         <v>25</v>
       </c>
       <c r="AE24" s="7" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="AF24" t="s">
         <v>25</v>
       </c>
-      <c r="AI24" s="26"/>
-      <c r="AJ24" s="26"/>
-      <c r="AK24" s="26"/>
-      <c r="AL24" s="26"/>
-      <c r="AM24" s="26"/>
-      <c r="AN24" s="26"/>
+      <c r="AI24" s="27"/>
+      <c r="AJ24" s="27"/>
+      <c r="AK24" s="27"/>
+      <c r="AL24" s="27"/>
+      <c r="AM24" s="27"/>
+      <c r="AN24" s="27"/>
     </row>
     <row r="25" spans="1:40" x14ac:dyDescent="0.25">
       <c r="AB25" s="15" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="AC25" t="s">
         <v>26</v>
       </c>
       <c r="AE25" s="7" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="AF25" t="s">
         <v>26</v>
       </c>
-      <c r="AI25" s="26"/>
-      <c r="AJ25" s="26"/>
-      <c r="AK25" s="26"/>
-      <c r="AL25" s="26"/>
-      <c r="AM25" s="26"/>
-      <c r="AN25" s="26"/>
+      <c r="AI25" s="27"/>
+      <c r="AJ25" s="27"/>
+      <c r="AK25" s="27"/>
+      <c r="AL25" s="27"/>
+      <c r="AM25" s="27"/>
+      <c r="AN25" s="27"/>
     </row>
     <row r="28" spans="1:40" x14ac:dyDescent="0.25">
       <c r="AB28" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="AC28" t="s">
         <v>37</v>
       </c>
-      <c r="AC28" t="s">
-        <v>38</v>
-      </c>
-      <c r="AI28" s="26" t="s">
-        <v>42</v>
-      </c>
-      <c r="AJ28" s="26"/>
-      <c r="AK28" s="26"/>
-      <c r="AL28" s="26"/>
-      <c r="AM28" s="26"/>
-      <c r="AN28" s="26"/>
+      <c r="AI28" s="27" t="s">
+        <v>41</v>
+      </c>
+      <c r="AJ28" s="27"/>
+      <c r="AK28" s="27"/>
+      <c r="AL28" s="27"/>
+      <c r="AM28" s="27"/>
+      <c r="AN28" s="27"/>
     </row>
     <row r="29" spans="1:40" x14ac:dyDescent="0.25">
       <c r="AB29" s="19" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="AC29" t="s">
-        <v>39</v>
-      </c>
-      <c r="AI29" s="26"/>
-      <c r="AJ29" s="26"/>
-      <c r="AK29" s="26"/>
-      <c r="AL29" s="26"/>
-      <c r="AM29" s="26"/>
-      <c r="AN29" s="26"/>
+        <v>38</v>
+      </c>
+      <c r="AI29" s="27"/>
+      <c r="AJ29" s="27"/>
+      <c r="AK29" s="27"/>
+      <c r="AL29" s="27"/>
+      <c r="AM29" s="27"/>
+      <c r="AN29" s="27"/>
     </row>
     <row r="30" spans="1:40" x14ac:dyDescent="0.25">
       <c r="AB30" s="19" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="AC30" t="s">
-        <v>40</v>
-      </c>
-      <c r="AI30" s="26"/>
-      <c r="AJ30" s="26"/>
-      <c r="AK30" s="26"/>
-      <c r="AL30" s="26"/>
-      <c r="AM30" s="26"/>
-      <c r="AN30" s="26"/>
+        <v>39</v>
+      </c>
+      <c r="AI30" s="27"/>
+      <c r="AJ30" s="27"/>
+      <c r="AK30" s="27"/>
+      <c r="AL30" s="27"/>
+      <c r="AM30" s="27"/>
+      <c r="AN30" s="27"/>
     </row>
     <row r="31" spans="1:40" x14ac:dyDescent="0.25">
       <c r="AB31" s="19" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="AC31" t="s">
-        <v>41</v>
-      </c>
-      <c r="AI31" s="26"/>
-      <c r="AJ31" s="26"/>
-      <c r="AK31" s="26"/>
-      <c r="AL31" s="26"/>
-      <c r="AM31" s="26"/>
-      <c r="AN31" s="26"/>
+        <v>40</v>
+      </c>
+      <c r="AI31" s="27"/>
+      <c r="AJ31" s="27"/>
+      <c r="AK31" s="27"/>
+      <c r="AL31" s="27"/>
+      <c r="AM31" s="27"/>
+      <c r="AN31" s="27"/>
     </row>
     <row r="32" spans="1:40" x14ac:dyDescent="0.25">
       <c r="AB32" s="20" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="AC32" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="33" spans="28:40" x14ac:dyDescent="0.25">
       <c r="AB33" s="20" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="AC33" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="46" spans="28:40" x14ac:dyDescent="0.25">
@@ -2793,14 +2841,14 @@
       <c r="AF46" t="s">
         <v>2</v>
       </c>
-      <c r="AI46" s="24" t="s">
+      <c r="AI46" s="25" t="s">
         <v>7</v>
       </c>
-      <c r="AJ46" s="24"/>
-      <c r="AK46" s="24"/>
-      <c r="AL46" s="24"/>
-      <c r="AM46" s="24"/>
-      <c r="AN46" s="24"/>
+      <c r="AJ46" s="25"/>
+      <c r="AK46" s="25"/>
+      <c r="AL46" s="25"/>
+      <c r="AM46" s="25"/>
+      <c r="AN46" s="25"/>
     </row>
     <row r="47" spans="28:40" x14ac:dyDescent="0.25">
       <c r="AB47" s="3" t="s">
@@ -2815,14 +2863,14 @@
       <c r="AF47" t="s">
         <v>3</v>
       </c>
-      <c r="AI47" s="24" t="s">
+      <c r="AI47" s="25" t="s">
         <v>8</v>
       </c>
-      <c r="AJ47" s="24"/>
-      <c r="AK47" s="24"/>
-      <c r="AL47" s="24"/>
-      <c r="AM47" s="24"/>
-      <c r="AN47" s="24"/>
+      <c r="AJ47" s="25"/>
+      <c r="AK47" s="25"/>
+      <c r="AL47" s="25"/>
+      <c r="AM47" s="25"/>
+      <c r="AN47" s="25"/>
     </row>
     <row r="48" spans="28:40" x14ac:dyDescent="0.25">
       <c r="AB48" s="12" t="s">
@@ -2837,14 +2885,14 @@
       <c r="AF48" t="s">
         <v>4</v>
       </c>
-      <c r="AI48" s="24" t="s">
+      <c r="AI48" s="25" t="s">
         <v>9</v>
       </c>
-      <c r="AJ48" s="24"/>
-      <c r="AK48" s="24"/>
-      <c r="AL48" s="24"/>
-      <c r="AM48" s="24"/>
-      <c r="AN48" s="24"/>
+      <c r="AJ48" s="25"/>
+      <c r="AK48" s="25"/>
+      <c r="AL48" s="25"/>
+      <c r="AM48" s="25"/>
+      <c r="AN48" s="25"/>
     </row>
   </sheetData>
   <mergeCells count="14">
@@ -2872,33 +2920,34 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M20" sqref="M20"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G18" sqref="G18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="4" max="4" width="20" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>45</v>
+      </c>
+      <c r="B1" t="s">
+        <v>46</v>
+      </c>
+      <c r="C1" t="s">
         <v>47</v>
       </c>
-      <c r="B1" t="s">
+      <c r="D1" t="s">
         <v>48</v>
       </c>
-      <c r="C1" t="s">
+      <c r="E1" t="s">
         <v>49</v>
       </c>
-      <c r="D1" t="s">
-        <v>50</v>
-      </c>
-      <c r="E1" t="s">
-        <v>51</v>
-      </c>
       <c r="F1" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="I1" s="21"/>
       <c r="L1" s="21"/>
@@ -2908,16 +2957,16 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C2" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="E2" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="F2" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="I2" s="22"/>
       <c r="J2" s="23">
@@ -2933,13 +2982,13 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="D3" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="E3" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="F3">
         <v>1</v>
@@ -2954,16 +3003,16 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C4" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="E4" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="F4" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="I4" s="21"/>
       <c r="J4" s="23"/>
@@ -2975,13 +3024,13 @@
         <v>3</v>
       </c>
       <c r="C5" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="E5" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="F5" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="I5" s="21"/>
       <c r="J5" s="23"/>
@@ -2993,13 +3042,13 @@
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C6" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="E6" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="F6">
         <v>2</v>
@@ -3018,16 +3067,16 @@
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C7" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="E7" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="F7" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="I7" s="21"/>
       <c r="J7" s="23"/>
@@ -3039,13 +3088,13 @@
         <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="C8" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="D8" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="I8" s="21"/>
       <c r="J8" s="23"/>
@@ -3057,13 +3106,13 @@
         <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="C9" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="D9" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="I9" s="21"/>
       <c r="J9" s="23"/>
@@ -3075,13 +3124,13 @@
         <v>8</v>
       </c>
       <c r="B10" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="C10" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="D10" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="I10" s="22"/>
       <c r="J10" s="23">
@@ -3097,13 +3146,13 @@
         <v>9</v>
       </c>
       <c r="B11" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="C11" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="D11" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="I11" s="21"/>
       <c r="L11" s="21"/>
@@ -3113,22 +3162,22 @@
         <v>10</v>
       </c>
       <c r="B12" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C12" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="D12" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="E12" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="F12">
         <v>3</v>
       </c>
       <c r="J12" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.25">
@@ -3136,13 +3185,13 @@
         <v>11</v>
       </c>
       <c r="B13" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="C13" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="D13" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.25">
@@ -3150,13 +3199,13 @@
         <v>12</v>
       </c>
       <c r="B14" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C14" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="E14" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="F14">
         <v>5</v>
@@ -3167,13 +3216,13 @@
         <v>13</v>
       </c>
       <c r="B15" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C15" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="E15" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="F15">
         <v>6</v>
@@ -3184,13 +3233,13 @@
         <v>14</v>
       </c>
       <c r="B16" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C16" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="E16" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="F16">
         <v>4</v>
@@ -3201,13 +3250,13 @@
         <v>15</v>
       </c>
       <c r="B17" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="E17" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="F17" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
@@ -3215,17 +3264,115 @@
         <v>16</v>
       </c>
       <c r="D18" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="E18" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="F18" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B10"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E17" sqref="E17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="9.140625" style="24"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="24" t="s">
+        <v>72</v>
+      </c>
+      <c r="B1" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="24">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="24">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="24">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="24">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="24">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" s="24" t="s">
+        <v>86</v>
+      </c>
+      <c r="B7" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" s="24" t="s">
+        <v>74</v>
+      </c>
+      <c r="B8" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" s="24" t="s">
+        <v>75</v>
+      </c>
+      <c r="B9" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" s="24" t="s">
+        <v>76</v>
+      </c>
+      <c r="B10" t="s">
+        <v>84</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>